<commit_message>
Many changes, forgot to push whoops
</commit_message>
<xml_diff>
--- a/Documentation/Timeline.xlsx
+++ b/Documentation/Timeline.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calum\Documents\University\MSciProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596F21A9-A319-4EA7-A56F-7E23A5E5C6E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C8D82B-2502-4C21-887A-3AD19856CBD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65587A43-3987-407F-8A48-552DF1445312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -91,13 +92,19 @@
   </si>
   <si>
     <t>Unreal Engine</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>05/10/2020: Need to fix arches on first window</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +116,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -265,26 +279,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -349,7 +343,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -357,26 +350,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,10 +379,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9933FF"/>
       <color rgb="FFFFA56D"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFCC99FF"/>
-      <color rgb="FF9933FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -702,387 +696,387 @@
   <dimension ref="A1:DN90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="Z61" sqref="Z61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" style="15" customWidth="1"/>
     <col min="2" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="15" width="10.42578125" style="8" customWidth="1"/>
+    <col min="14" max="15" width="10.42578125" style="7" customWidth="1"/>
     <col min="16" max="20" width="10.42578125" customWidth="1"/>
-    <col min="21" max="22" width="10.42578125" style="8" customWidth="1"/>
+    <col min="21" max="22" width="10.42578125" style="7" customWidth="1"/>
     <col min="23" max="97" width="10.42578125" customWidth="1"/>
     <col min="98" max="98" width="11.5703125" customWidth="1"/>
     <col min="99" max="118" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:118" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="17">
         <v>44088</v>
       </c>
-      <c r="C1" s="22">
+      <c r="C1" s="17">
         <v>44089</v>
       </c>
-      <c r="D1" s="22">
+      <c r="D1" s="17">
         <v>44090</v>
       </c>
-      <c r="E1" s="22">
+      <c r="E1" s="17">
         <v>44091</v>
       </c>
-      <c r="F1" s="22">
+      <c r="F1" s="17">
         <v>44092</v>
       </c>
-      <c r="G1" s="22">
+      <c r="G1" s="17">
         <v>44093</v>
       </c>
-      <c r="H1" s="22">
+      <c r="H1" s="17">
         <v>44094</v>
       </c>
-      <c r="I1" s="22">
+      <c r="I1" s="17">
         <v>44095</v>
       </c>
-      <c r="J1" s="22">
+      <c r="J1" s="17">
         <v>44096</v>
       </c>
-      <c r="K1" s="22">
+      <c r="K1" s="17">
         <v>44097</v>
       </c>
-      <c r="L1" s="22">
+      <c r="L1" s="17">
         <v>44098</v>
       </c>
-      <c r="M1" s="22">
+      <c r="M1" s="17">
         <v>44099</v>
       </c>
-      <c r="N1" s="22">
+      <c r="N1" s="17">
         <v>44100</v>
       </c>
-      <c r="O1" s="22">
+      <c r="O1" s="17">
         <v>44101</v>
       </c>
-      <c r="P1" s="22">
+      <c r="P1" s="17">
         <v>44102</v>
       </c>
-      <c r="Q1" s="22">
+      <c r="Q1" s="17">
         <v>44103</v>
       </c>
-      <c r="R1" s="22">
+      <c r="R1" s="17">
         <v>44104</v>
       </c>
-      <c r="S1" s="22">
+      <c r="S1" s="17">
         <v>44105</v>
       </c>
-      <c r="T1" s="22">
+      <c r="T1" s="17">
         <v>44106</v>
       </c>
-      <c r="U1" s="22">
+      <c r="U1" s="17">
         <v>44107</v>
       </c>
-      <c r="V1" s="22">
+      <c r="V1" s="17">
         <v>44108</v>
       </c>
-      <c r="W1" s="22">
+      <c r="W1" s="17">
         <v>44109</v>
       </c>
-      <c r="X1" s="22">
+      <c r="X1" s="17">
         <v>44110</v>
       </c>
-      <c r="Y1" s="22">
+      <c r="Y1" s="17">
         <v>44111</v>
       </c>
-      <c r="Z1" s="22">
+      <c r="Z1" s="17">
         <v>44112</v>
       </c>
-      <c r="AA1" s="22">
+      <c r="AA1" s="17">
         <v>44113</v>
       </c>
-      <c r="AB1" s="22">
+      <c r="AB1" s="17">
         <v>44114</v>
       </c>
-      <c r="AC1" s="22">
+      <c r="AC1" s="17">
         <v>44115</v>
       </c>
-      <c r="AD1" s="22">
+      <c r="AD1" s="17">
         <v>44116</v>
       </c>
-      <c r="AE1" s="22">
+      <c r="AE1" s="17">
         <v>44117</v>
       </c>
-      <c r="AF1" s="22">
+      <c r="AF1" s="17">
         <v>44118</v>
       </c>
-      <c r="AG1" s="22">
+      <c r="AG1" s="17">
         <v>44119</v>
       </c>
-      <c r="AH1" s="22">
+      <c r="AH1" s="17">
         <v>44120</v>
       </c>
-      <c r="AI1" s="22">
+      <c r="AI1" s="17">
         <v>44121</v>
       </c>
-      <c r="AJ1" s="22">
+      <c r="AJ1" s="17">
         <v>44122</v>
       </c>
-      <c r="AK1" s="22">
+      <c r="AK1" s="17">
         <v>44123</v>
       </c>
-      <c r="AL1" s="22">
+      <c r="AL1" s="17">
         <v>44124</v>
       </c>
-      <c r="AM1" s="22">
+      <c r="AM1" s="17">
         <v>44125</v>
       </c>
-      <c r="AN1" s="22">
+      <c r="AN1" s="17">
         <v>44126</v>
       </c>
-      <c r="AO1" s="22">
+      <c r="AO1" s="17">
         <v>44127</v>
       </c>
-      <c r="AP1" s="22">
+      <c r="AP1" s="17">
         <v>44128</v>
       </c>
-      <c r="AQ1" s="22">
+      <c r="AQ1" s="17">
         <v>44129</v>
       </c>
-      <c r="AR1" s="22">
+      <c r="AR1" s="17">
         <v>44130</v>
       </c>
-      <c r="AS1" s="22">
+      <c r="AS1" s="17">
         <v>44131</v>
       </c>
-      <c r="AT1" s="22">
+      <c r="AT1" s="17">
         <v>44132</v>
       </c>
-      <c r="AU1" s="22">
+      <c r="AU1" s="17">
         <v>44133</v>
       </c>
-      <c r="AV1" s="22">
+      <c r="AV1" s="17">
         <v>44134</v>
       </c>
-      <c r="AW1" s="22">
+      <c r="AW1" s="17">
         <v>44135</v>
       </c>
-      <c r="AX1" s="22">
+      <c r="AX1" s="17">
         <v>44136</v>
       </c>
-      <c r="AY1" s="22">
+      <c r="AY1" s="17">
         <v>44137</v>
       </c>
-      <c r="AZ1" s="22">
+      <c r="AZ1" s="17">
         <v>44138</v>
       </c>
-      <c r="BA1" s="22">
+      <c r="BA1" s="17">
         <v>44139</v>
       </c>
-      <c r="BB1" s="22">
+      <c r="BB1" s="17">
         <v>44140</v>
       </c>
-      <c r="BC1" s="22">
+      <c r="BC1" s="17">
         <v>44141</v>
       </c>
-      <c r="BD1" s="22">
+      <c r="BD1" s="17">
         <v>44142</v>
       </c>
-      <c r="BE1" s="22">
+      <c r="BE1" s="17">
         <v>44143</v>
       </c>
-      <c r="BF1" s="22">
+      <c r="BF1" s="17">
         <v>44144</v>
       </c>
-      <c r="BG1" s="22">
+      <c r="BG1" s="17">
         <v>44145</v>
       </c>
-      <c r="BH1" s="22">
+      <c r="BH1" s="17">
         <v>44146</v>
       </c>
-      <c r="BI1" s="22">
+      <c r="BI1" s="17">
         <v>44147</v>
       </c>
-      <c r="BJ1" s="22">
+      <c r="BJ1" s="17">
         <v>44148</v>
       </c>
-      <c r="BK1" s="22">
+      <c r="BK1" s="17">
         <v>44149</v>
       </c>
-      <c r="BL1" s="22">
+      <c r="BL1" s="17">
         <v>44150</v>
       </c>
-      <c r="BM1" s="22">
+      <c r="BM1" s="17">
         <v>44151</v>
       </c>
-      <c r="BN1" s="22">
+      <c r="BN1" s="17">
         <v>44152</v>
       </c>
-      <c r="BO1" s="22">
+      <c r="BO1" s="17">
         <v>44153</v>
       </c>
-      <c r="BP1" s="22">
+      <c r="BP1" s="17">
         <v>44154</v>
       </c>
-      <c r="BQ1" s="22">
+      <c r="BQ1" s="17">
         <v>44155</v>
       </c>
-      <c r="BR1" s="22">
+      <c r="BR1" s="17">
         <v>44156</v>
       </c>
-      <c r="BS1" s="22">
+      <c r="BS1" s="17">
         <v>44157</v>
       </c>
-      <c r="BT1" s="22">
+      <c r="BT1" s="17">
         <v>44158</v>
       </c>
-      <c r="BU1" s="22">
+      <c r="BU1" s="17">
         <v>44159</v>
       </c>
-      <c r="BV1" s="22">
+      <c r="BV1" s="17">
         <v>44160</v>
       </c>
-      <c r="BW1" s="22">
+      <c r="BW1" s="17">
         <v>44161</v>
       </c>
-      <c r="BX1" s="22">
+      <c r="BX1" s="17">
         <v>44162</v>
       </c>
-      <c r="BY1" s="22">
+      <c r="BY1" s="17">
         <v>44163</v>
       </c>
-      <c r="BZ1" s="22">
+      <c r="BZ1" s="17">
         <v>44164</v>
       </c>
-      <c r="CA1" s="22">
+      <c r="CA1" s="17">
         <v>44165</v>
       </c>
-      <c r="CB1" s="22">
+      <c r="CB1" s="17">
         <v>44166</v>
       </c>
-      <c r="CC1" s="22">
+      <c r="CC1" s="17">
         <v>44167</v>
       </c>
-      <c r="CD1" s="22">
+      <c r="CD1" s="17">
         <v>44168</v>
       </c>
-      <c r="CE1" s="22">
+      <c r="CE1" s="17">
         <v>44169</v>
       </c>
-      <c r="CF1" s="22">
+      <c r="CF1" s="17">
         <v>44170</v>
       </c>
-      <c r="CG1" s="22">
+      <c r="CG1" s="17">
         <v>44171</v>
       </c>
-      <c r="CH1" s="22">
+      <c r="CH1" s="17">
         <v>44172</v>
       </c>
-      <c r="CI1" s="22">
+      <c r="CI1" s="17">
         <v>44173</v>
       </c>
-      <c r="CJ1" s="22">
+      <c r="CJ1" s="17">
         <v>44174</v>
       </c>
-      <c r="CK1" s="22">
+      <c r="CK1" s="17">
         <v>44175</v>
       </c>
-      <c r="CL1" s="22">
+      <c r="CL1" s="17">
         <v>44176</v>
       </c>
-      <c r="CM1" s="22">
+      <c r="CM1" s="17">
         <v>44177</v>
       </c>
-      <c r="CN1" s="22">
+      <c r="CN1" s="17">
         <v>44178</v>
       </c>
-      <c r="CO1" s="22">
+      <c r="CO1" s="17">
         <v>44179</v>
       </c>
-      <c r="CP1" s="22">
+      <c r="CP1" s="17">
         <v>44180</v>
       </c>
-      <c r="CQ1" s="22">
+      <c r="CQ1" s="17">
         <v>44181</v>
       </c>
-      <c r="CR1" s="22">
+      <c r="CR1" s="17">
         <v>44182</v>
       </c>
-      <c r="CS1" s="22">
+      <c r="CS1" s="17">
         <v>44183</v>
       </c>
-      <c r="CT1" s="22">
+      <c r="CT1" s="17">
         <v>44184</v>
       </c>
-      <c r="CU1" s="22">
+      <c r="CU1" s="17">
         <v>44185</v>
       </c>
-      <c r="CV1" s="22">
+      <c r="CV1" s="17">
         <v>44186</v>
       </c>
-      <c r="CW1" s="22">
+      <c r="CW1" s="17">
         <v>44187</v>
       </c>
-      <c r="CX1" s="22">
+      <c r="CX1" s="17">
         <v>44188</v>
       </c>
-      <c r="CY1" s="22">
+      <c r="CY1" s="17">
         <v>44189</v>
       </c>
-      <c r="CZ1" s="22">
+      <c r="CZ1" s="17">
         <v>44190</v>
       </c>
-      <c r="DA1" s="22">
+      <c r="DA1" s="17">
         <v>44191</v>
       </c>
-      <c r="DB1" s="22">
+      <c r="DB1" s="17">
         <v>44192</v>
       </c>
-      <c r="DC1" s="22">
+      <c r="DC1" s="17">
         <v>44193</v>
       </c>
-      <c r="DD1" s="22">
+      <c r="DD1" s="17">
         <v>44194</v>
       </c>
-      <c r="DE1" s="22">
+      <c r="DE1" s="17">
         <v>44195</v>
       </c>
-      <c r="DF1" s="22">
+      <c r="DF1" s="17">
         <v>44196</v>
       </c>
-      <c r="DG1" s="22">
+      <c r="DG1" s="17">
         <v>44197</v>
       </c>
-      <c r="DH1" s="22">
+      <c r="DH1" s="17">
         <v>44198</v>
       </c>
-      <c r="DI1" s="22">
+      <c r="DI1" s="17">
         <v>44199</v>
       </c>
-      <c r="DJ1" s="22">
+      <c r="DJ1" s="17">
         <v>44200</v>
       </c>
-      <c r="DK1" s="22">
+      <c r="DK1" s="17">
         <v>44201</v>
       </c>
-      <c r="DL1" s="22">
+      <c r="DL1" s="17">
         <v>44202</v>
       </c>
-      <c r="DM1" s="22">
+      <c r="DM1" s="17">
         <v>44203</v>
       </c>
-      <c r="DN1" s="23">
+      <c r="DN1" s="18">
         <v>44204</v>
       </c>
     </row>
-    <row r="2" spans="1:118" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:118" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
@@ -1094,30 +1088,30 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6"/>
-      <c r="P4" s="12"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
@@ -1132,17 +1126,17 @@
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:118" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:118" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3"/>
@@ -1157,96 +1151,150 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="3"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="1"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="2"/>
-      <c r="Z10" s="14"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="34"/>
     </row>
     <row r="11" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="16"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="2"/>
     </row>
     <row r="12" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="7"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
     </row>
     <row r="13" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="7"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="2"/>
     </row>
     <row r="14" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="V14" s="18"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="7"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="2"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="2"/>
     </row>
     <row r="15" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="W15" s="1"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="2"/>
-    </row>
-    <row r="60" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="60" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="13"/>
+      <c r="C61" s="12"/>
+      <c r="Z61" s="12"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="13"/>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z63" s="13"/>
+      <c r="E62" s="12"/>
+      <c r="Z62" s="12"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z64" s="14"/>
-    </row>
-    <row r="66" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="31" t="s">
+      <c r="Z64" s="13"/>
+    </row>
+    <row r="66" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="33" t="s">
+    <row r="90" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="28" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1254,4 +1302,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB9C1F8-1EE4-4BB1-96F0-5ACB4EC13C2A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="97.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>